<commit_message>
Added some stats to the spreadsheet.
</commit_message>
<xml_diff>
--- a/Graphics/20200528/20200528_Kosovo_COVID.xlsx
+++ b/Graphics/20200528/20200528_Kosovo_COVID.xlsx
@@ -366,7 +366,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,12 +437,22 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>Positive_2D_Mean</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>Tested_Positive_Ratio</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Active_Infections</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Positive_3D_Mean</t>
         </is>
       </c>
     </row>
@@ -494,6 +504,12 @@
       <c r="O2" t="n">
         <v>14</v>
       </c>
+      <c r="P2" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -538,10 +554,16 @@
         <v>-0.07142857142857142</v>
       </c>
       <c r="N3" t="n">
+        <v>8.892857142857142</v>
+      </c>
+      <c r="O3" t="n">
         <v>3.273958952934351</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>245</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>9.333333333333332</v>
       </c>
     </row>
     <row r="4">
@@ -587,10 +609,16 @@
         <v>0.2672612419124244</v>
       </c>
       <c r="N4" t="n">
+        <v>4.93097966326778</v>
+      </c>
+      <c r="O4" t="n">
         <v>2.574352377869752</v>
       </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
         <v>12.62476199318686</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>4.51209201579205</v>
       </c>
     </row>
     <row r="5">
@@ -636,10 +664,16 @@
         <v>-1</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
         <v>220</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>3.666666666666667</v>
       </c>
     </row>
     <row r="6">
@@ -685,10 +719,16 @@
         <v>0</v>
       </c>
       <c r="N6" t="n">
+        <v>5</v>
+      </c>
+      <c r="O6" t="n">
         <v>0.8922413793103449</v>
       </c>
-      <c r="O6" t="n">
+      <c r="P6" t="n">
         <v>236.25</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>5.333333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -734,10 +774,16 @@
         <v>0</v>
       </c>
       <c r="N7" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="O7" t="n">
         <v>2.9672411685613</v>
       </c>
-      <c r="O7" t="n">
+      <c r="P7" t="n">
         <v>247</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>9.5</v>
       </c>
     </row>
     <row r="8">
@@ -783,10 +829,16 @@
         <v>0</v>
       </c>
       <c r="N8" t="n">
+        <v>13.75</v>
+      </c>
+      <c r="O8" t="n">
         <v>5.297651272227544</v>
       </c>
-      <c r="O8" t="n">
+      <c r="P8" t="n">
         <v>252</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -832,10 +884,236 @@
         <v>0</v>
       </c>
       <c r="N9" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="O9" t="n">
         <v>7.865168539325842</v>
       </c>
-      <c r="O9" t="n">
+      <c r="P9" t="n">
         <v>265</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>var</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4773.758241758242</v>
+      </c>
+      <c r="C10" t="n">
+        <v>59.32417582417582</v>
+      </c>
+      <c r="D10" t="n">
+        <v>70.21978021978022</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.07142857142857142</v>
+      </c>
+      <c r="F10" t="n">
+        <v>899542.5274725276</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.1928082958766484</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1102.994505494506</v>
+      </c>
+      <c r="I10" t="n">
+        <v>39.38147481075434</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1430.686813186813</v>
+      </c>
+      <c r="K10" t="n">
+        <v>32.38696892707112</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.1813186813186813</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.07142857142857142</v>
+      </c>
+      <c r="N10" t="n">
+        <v>24.31456043956043</v>
+      </c>
+      <c r="O10" t="n">
+        <v>6.627290165443648</v>
+      </c>
+      <c r="P10" t="n">
+        <v>159.3846153846154</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>20.35897435897436</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>skew</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.8790319229385586</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.7129435877424485</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.5702900284721719</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3.741657386773941</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-0.06755170123791036</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.4591203867726038</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-0.3374217857993511</v>
+      </c>
+      <c r="I11" t="n">
+        <v>2.449496305798799</v>
+      </c>
+      <c r="J11" t="n">
+        <v>-0.9826348506355927</v>
+      </c>
+      <c r="K11" t="n">
+        <v>3.662976687888275</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1.565623981413936</v>
+      </c>
+      <c r="M11" t="n">
+        <v>-3.741657386773941</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.1482013660683004</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.3549571738761034</v>
+      </c>
+      <c r="P11" t="n">
+        <v>-0.2432478289573481</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.3890407428082802</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>kurt</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1.615578540030924</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-0.6699093863710988</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-1.41606490080999</v>
+      </c>
+      <c r="E12" t="n">
+        <v>14</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-1.009803974186463</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-0.5094325902720964</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-0.928822738263023</v>
+      </c>
+      <c r="I12" t="n">
+        <v>5.296962645784837</v>
+      </c>
+      <c r="J12" t="n">
+        <v>-0.3621042896467785</v>
+      </c>
+      <c r="K12" t="n">
+        <v>13.57376670881802</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.5013774104682991</v>
+      </c>
+      <c r="M12" t="n">
+        <v>14</v>
+      </c>
+      <c r="N12" t="n">
+        <v>-1.525746016243464</v>
+      </c>
+      <c r="O12" t="n">
+        <v>-1.1145158880739</v>
+      </c>
+      <c r="P12" t="n">
+        <v>-0.09783867976435534</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>-1.07856996322122</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>mad</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>50.61224489795919</v>
+      </c>
+      <c r="C13" t="n">
+        <v>6.163265306122448</v>
+      </c>
+      <c r="D13" t="n">
+        <v>7.326530612244901</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.1326530612244898</v>
+      </c>
+      <c r="F13" t="n">
+        <v>778.1428571428571</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.3336749970236609</v>
+      </c>
+      <c r="H13" t="n">
+        <v>27.48979591836735</v>
+      </c>
+      <c r="I13" t="n">
+        <v>4.09821058858326</v>
+      </c>
+      <c r="J13" t="n">
+        <v>30.80612244897959</v>
+      </c>
+      <c r="K13" t="n">
+        <v>2.807339848774958</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.3367346938775516</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.1326530612244898</v>
+      </c>
+      <c r="N13" t="n">
+        <v>4.306122448979592</v>
+      </c>
+      <c r="O13" t="n">
+        <v>2.160410644545148</v>
+      </c>
+      <c r="P13" t="n">
+        <v>9.571428571428571</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>3.761904761904763</v>
       </c>
     </row>
   </sheetData>
@@ -849,7 +1127,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -920,12 +1198,22 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>Positive_2D_Mean</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>Tested_Positive_Ratio</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Active_Infections</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Positive_3D_Mean</t>
         </is>
       </c>
     </row>
@@ -972,11 +1260,17 @@
         <v>92</v>
       </c>
       <c r="N2" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O2" t="n">
         <v>92</v>
       </c>
+      <c r="P2" t="n">
+        <v>92</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1021,10 +1315,16 @@
         <v>-0.1340579710144928</v>
       </c>
       <c r="N3" t="n">
+        <v>11.51098901098901</v>
+      </c>
+      <c r="O3" t="n">
         <v>6.947593626131382</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>208.8478260869565</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>11.6037037037037</v>
       </c>
     </row>
     <row r="4">
@@ -1070,10 +1370,16 @@
         <v>0.359112263912071</v>
       </c>
       <c r="N4" t="n">
+        <v>12.12022598386177</v>
+      </c>
+      <c r="O4" t="n">
         <v>7.455358834485447</v>
       </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
         <v>182.41487159724</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>11.31336580350234</v>
       </c>
     </row>
     <row r="5">
@@ -1124,6 +1430,12 @@
       <c r="O5" t="n">
         <v>0</v>
       </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1168,10 +1480,16 @@
         <v>0</v>
       </c>
       <c r="N6" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="O6" t="n">
         <v>0.7974137931034483</v>
       </c>
-      <c r="O6" t="n">
+      <c r="P6" t="n">
         <v>23.25</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>3.083333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -1217,10 +1535,16 @@
         <v>0</v>
       </c>
       <c r="N7" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="O7" t="n">
         <v>4.433800049127978</v>
       </c>
-      <c r="O7" t="n">
+      <c r="P7" t="n">
         <v>218.5</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>8.166666666666668</v>
       </c>
     </row>
     <row r="8">
@@ -1266,10 +1590,16 @@
         <v>0</v>
       </c>
       <c r="N8" t="n">
+        <v>16</v>
+      </c>
+      <c r="O8" t="n">
         <v>10.55479249530241</v>
       </c>
-      <c r="O8" t="n">
+      <c r="P8" t="n">
         <v>315.75</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>16.58333333333333</v>
       </c>
     </row>
     <row r="9">
@@ -1315,10 +1645,236 @@
         <v>1</v>
       </c>
       <c r="N9" t="n">
+        <v>56</v>
+      </c>
+      <c r="O9" t="n">
         <v>31.6</v>
       </c>
-      <c r="O9" t="n">
+      <c r="P9" t="n">
         <v>597</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>var</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>11807.91722408027</v>
+      </c>
+      <c r="C10" t="n">
+        <v>194.2847587195414</v>
+      </c>
+      <c r="D10" t="n">
+        <v>215.9239130434783</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.4859053989488771</v>
+      </c>
+      <c r="F10" t="n">
+        <v>21055138.3940516</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1.686184363474859</v>
+      </c>
+      <c r="H10" t="n">
+        <v>160077.7786669852</v>
+      </c>
+      <c r="I10" t="n">
+        <v>9.980250705333088</v>
+      </c>
+      <c r="J10" t="n">
+        <v>86813.37255136172</v>
+      </c>
+      <c r="K10" t="n">
+        <v>19.78736426783364</v>
+      </c>
+      <c r="L10" t="n">
+        <v>146.7523889154323</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.1289616180920529</v>
+      </c>
+      <c r="N10" t="n">
+        <v>146.8998778998779</v>
+      </c>
+      <c r="O10" t="n">
+        <v>55.5823753509402</v>
+      </c>
+      <c r="P10" t="n">
+        <v>33275.18537983756</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>127.9922458038563</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>skew</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.09122853463491004</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1.964913941679069</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2.750069125669569</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2.439393697797227</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.6185095503958902</v>
+      </c>
+      <c r="G11" t="n">
+        <v>5.313599315506452</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.261774815811131</v>
+      </c>
+      <c r="I11" t="n">
+        <v>3.963686232939136</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1.003370182137258</v>
+      </c>
+      <c r="K11" t="n">
+        <v>5.934997801066514</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.364520324367599</v>
+      </c>
+      <c r="M11" t="n">
+        <v>-1.431382368997289</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1.457680873179369</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1.369978524472223</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.5369279706280452</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>1.149132626998142</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>kurt</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>-0.9499799192292637</v>
+      </c>
+      <c r="C12" t="n">
+        <v>5.359347580456541</v>
+      </c>
+      <c r="D12" t="n">
+        <v>9.634455957030847</v>
+      </c>
+      <c r="E12" t="n">
+        <v>5.887565999988205</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-1.06137922676375</v>
+      </c>
+      <c r="G12" t="n">
+        <v>38.11898556705106</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-1.655855966802221</v>
+      </c>
+      <c r="I12" t="n">
+        <v>18.1125851987996</v>
+      </c>
+      <c r="J12" t="n">
+        <v>-0.7018258601576606</v>
+      </c>
+      <c r="K12" t="n">
+        <v>38.73286701170495</v>
+      </c>
+      <c r="L12" t="n">
+        <v>-1.628448426936274</v>
+      </c>
+      <c r="M12" t="n">
+        <v>2.587520685325253</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1.950177908577426</v>
+      </c>
+      <c r="O12" t="n">
+        <v>1.405593232564954</v>
+      </c>
+      <c r="P12" t="n">
+        <v>-0.8409150091939113</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.5544138509129124</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>mad</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>94.07443289224948</v>
+      </c>
+      <c r="C13" t="n">
+        <v>10.52741020793951</v>
+      </c>
+      <c r="D13" t="n">
+        <v>10.12240075614366</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.503308128544424</v>
+      </c>
+      <c r="F13" t="n">
+        <v>4023.826559546314</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.6918148693158707</v>
+      </c>
+      <c r="H13" t="n">
+        <v>371.3426275992438</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1.725024363443752</v>
+      </c>
+      <c r="J13" t="n">
+        <v>252.8908317580341</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1.754261873720469</v>
+      </c>
+      <c r="L13" t="n">
+        <v>11.19825141776938</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.2461405166981726</v>
+      </c>
+      <c r="N13" t="n">
+        <v>9.299239222316148</v>
+      </c>
+      <c r="O13" t="n">
+        <v>5.774656590634603</v>
+      </c>
+      <c r="P13" t="n">
+        <v>152.0685255198491</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>8.906831275720165</v>
       </c>
     </row>
   </sheetData>
@@ -1332,7 +1888,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O93"/>
+  <dimension ref="A1:Q93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1378,40 +1934,50 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>Positive_2D_Mean</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Positive_3D_Mean</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>Recovered_Raw</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Recovered_Cum</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Recovered_Delta</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Died_Raw</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Died_Cum</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Died_Delta</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Tested_Positive_Ratio</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Active_Infections</t>
         </is>
@@ -1463,6 +2029,12 @@
       <c r="O2" t="n">
         <v>0</v>
       </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -1510,6 +2082,12 @@
       <c r="O3" t="n">
         <v>0</v>
       </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -1557,6 +2135,12 @@
       <c r="O4" t="n">
         <v>0</v>
       </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -1604,6 +2188,12 @@
       <c r="O5" t="n">
         <v>0</v>
       </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -1651,6 +2241,12 @@
       <c r="O6" t="n">
         <v>0</v>
       </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -1698,6 +2294,12 @@
       <c r="O7" t="n">
         <v>0</v>
       </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -1745,6 +2347,12 @@
       <c r="O8" t="n">
         <v>0</v>
       </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -1792,6 +2400,12 @@
       <c r="O9" t="n">
         <v>0</v>
       </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -1839,6 +2453,12 @@
       <c r="O10" t="n">
         <v>0</v>
       </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -1886,6 +2506,12 @@
       <c r="O11" t="n">
         <v>0</v>
       </c>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -1933,6 +2559,12 @@
       <c r="O12" t="n">
         <v>0</v>
       </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -1980,6 +2612,12 @@
       <c r="O13" t="n">
         <v>0</v>
       </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -2027,6 +2665,12 @@
       <c r="O14" t="n">
         <v>0</v>
       </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -2074,6 +2718,12 @@
       <c r="O15" t="n">
         <v>0</v>
       </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -2121,6 +2771,12 @@
       <c r="O16" t="n">
         <v>0</v>
       </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -2168,6 +2824,12 @@
       <c r="O17" t="n">
         <v>0</v>
       </c>
+      <c r="P17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -2192,10 +2854,10 @@
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J18" t="n">
         <v>0</v>
@@ -2210,9 +2872,15 @@
         <v>0</v>
       </c>
       <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" t="n">
         <v>7.692307692307693</v>
       </c>
-      <c r="O18" t="n">
+      <c r="Q18" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2239,10 +2907,10 @@
         <v>0.5</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
@@ -2257,9 +2925,15 @@
         <v>0</v>
       </c>
       <c r="N19" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" t="n">
         <v>3.03030303030303</v>
       </c>
-      <c r="O19" t="n">
+      <c r="Q19" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2286,10 +2960,10 @@
         <v>1.666666666666667</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="J20" t="n">
         <v>0</v>
@@ -2304,9 +2978,15 @@
         <v>0</v>
       </c>
       <c r="N20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" t="n">
         <v>29.62962962962963</v>
       </c>
-      <c r="O20" t="n">
+      <c r="Q20" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2333,10 +3013,10 @@
         <v>-0.625</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="J21" t="n">
         <v>0</v>
@@ -2351,9 +3031,15 @@
         <v>0</v>
       </c>
       <c r="N21" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" t="n">
         <v>12.5</v>
       </c>
-      <c r="O21" t="n">
+      <c r="Q21" t="n">
         <v>16</v>
       </c>
     </row>
@@ -2380,10 +3066,10 @@
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="J22" t="n">
         <v>0</v>
@@ -2398,9 +3084,15 @@
         <v>0</v>
       </c>
       <c r="N22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" t="n">
         <v>23.07692307692308</v>
       </c>
-      <c r="O22" t="n">
+      <c r="Q22" t="n">
         <v>19</v>
       </c>
     </row>
@@ -2427,10 +3119,10 @@
         <v>-0.6666666666666667</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="J23" t="n">
         <v>0</v>
@@ -2445,9 +3137,15 @@
         <v>0</v>
       </c>
       <c r="N23" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" t="n">
         <v>2.857142857142857</v>
       </c>
-      <c r="O23" t="n">
+      <c r="Q23" t="n">
         <v>20</v>
       </c>
     </row>
@@ -2474,10 +3172,10 @@
         <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="J24" t="n">
         <v>0</v>
@@ -2492,9 +3190,15 @@
         <v>0</v>
       </c>
       <c r="N24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" t="n">
         <v>4.761904761904762</v>
       </c>
-      <c r="O24" t="n">
+      <c r="Q24" t="n">
         <v>21</v>
       </c>
     </row>
@@ -2521,10 +3225,10 @@
         <v>2</v>
       </c>
       <c r="H25" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="J25" t="n">
         <v>0</v>
@@ -2539,9 +3243,15 @@
         <v>0</v>
       </c>
       <c r="N25" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" t="n">
         <v>3.896103896103896</v>
       </c>
-      <c r="O25" t="n">
+      <c r="Q25" t="n">
         <v>24</v>
       </c>
     </row>
@@ -2568,10 +3278,10 @@
         <v>1.333333333333333</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>3.666666666666667</v>
       </c>
       <c r="J26" t="n">
         <v>0</v>
@@ -2586,9 +3296,15 @@
         <v>0</v>
       </c>
       <c r="N26" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0</v>
+      </c>
+      <c r="P26" t="n">
         <v>4.666666666666667</v>
       </c>
-      <c r="O26" t="n">
+      <c r="Q26" t="n">
         <v>31</v>
       </c>
     </row>
@@ -2615,27 +3331,33 @@
         <v>-0.7142857142857143</v>
       </c>
       <c r="H27" t="n">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J27" t="n">
         <v>0</v>
       </c>
       <c r="K27" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" t="n">
         <v>1</v>
       </c>
-      <c r="L27" t="n">
+      <c r="N27" t="n">
         <v>1</v>
       </c>
-      <c r="M27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N27" t="n">
+      <c r="O27" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" t="n">
         <v>20</v>
       </c>
-      <c r="O27" t="n">
+      <c r="Q27" t="n">
         <v>33</v>
       </c>
     </row>
@@ -2662,10 +3384,10 @@
         <v>13</v>
       </c>
       <c r="H28" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>12.33333333333333</v>
       </c>
       <c r="J28" t="n">
         <v>0</v>
@@ -2674,15 +3396,21 @@
         <v>0</v>
       </c>
       <c r="L28" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
         <v>1</v>
       </c>
-      <c r="M28" t="n">
+      <c r="O28" t="n">
         <v>-1</v>
       </c>
-      <c r="N28" t="n">
+      <c r="P28" t="n">
         <v>24.7787610619469</v>
       </c>
-      <c r="O28" t="n">
+      <c r="Q28" t="n">
         <v>61</v>
       </c>
     </row>
@@ -2709,10 +3437,10 @@
         <v>-0.9285714285714286</v>
       </c>
       <c r="H29" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>10.66666666666667</v>
       </c>
       <c r="J29" t="n">
         <v>0</v>
@@ -2721,15 +3449,21 @@
         <v>0</v>
       </c>
       <c r="L29" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
         <v>1</v>
       </c>
-      <c r="M29" t="n">
-        <v>0</v>
-      </c>
-      <c r="N29" t="n">
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" t="n">
         <v>4.761904761904762</v>
       </c>
-      <c r="O29" t="n">
+      <c r="Q29" t="n">
         <v>63</v>
       </c>
     </row>
@@ -2756,10 +3490,10 @@
         <v>3</v>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>12.66666666666667</v>
       </c>
       <c r="J30" t="n">
         <v>0</v>
@@ -2768,15 +3502,21 @@
         <v>0</v>
       </c>
       <c r="L30" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="n">
         <v>1</v>
       </c>
-      <c r="M30" t="n">
-        <v>0</v>
-      </c>
-      <c r="N30" t="n">
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
         <v>23.52941176470588</v>
       </c>
-      <c r="O30" t="n">
+      <c r="Q30" t="n">
         <v>71</v>
       </c>
     </row>
@@ -2803,27 +3543,33 @@
         <v>0.875</v>
       </c>
       <c r="H31" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="I31" t="n">
+        <v>8.333333333333334</v>
+      </c>
+      <c r="J31" t="n">
         <v>1</v>
       </c>
-      <c r="I31" t="n">
+      <c r="K31" t="n">
         <v>1</v>
       </c>
-      <c r="J31" t="n">
-        <v>0</v>
-      </c>
-      <c r="K31" t="n">
-        <v>0</v>
-      </c>
       <c r="L31" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="n">
         <v>1</v>
       </c>
-      <c r="M31" t="n">
-        <v>0</v>
-      </c>
-      <c r="N31" t="n">
+      <c r="O31" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" t="n">
         <v>12.60504201680672</v>
       </c>
-      <c r="O31" t="n">
+      <c r="Q31" t="n">
         <v>85</v>
       </c>
     </row>
@@ -2850,27 +3596,33 @@
         <v>-0.8666666666666667</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="I32" t="n">
+        <v>8.333333333333334</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" t="n">
         <v>1</v>
       </c>
-      <c r="J32" t="n">
+      <c r="L32" t="n">
         <v>-1</v>
       </c>
-      <c r="K32" t="n">
-        <v>0</v>
-      </c>
-      <c r="L32" t="n">
+      <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
         <v>1</v>
       </c>
-      <c r="M32" t="n">
-        <v>0</v>
-      </c>
-      <c r="N32" t="n">
+      <c r="O32" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" t="n">
         <v>1.886792452830189</v>
       </c>
-      <c r="O32" t="n">
+      <c r="Q32" t="n">
         <v>87</v>
       </c>
     </row>
@@ -2897,27 +3649,33 @@
         <v>0.5</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="I33" t="n">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" t="n">
         <v>1</v>
       </c>
-      <c r="J33" t="n">
-        <v>0</v>
-      </c>
-      <c r="K33" t="n">
-        <v>0</v>
-      </c>
       <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
         <v>1</v>
       </c>
-      <c r="M33" t="n">
-        <v>0</v>
-      </c>
-      <c r="N33" t="n">
+      <c r="O33" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" t="n">
         <v>6.521739130434782</v>
       </c>
-      <c r="O33" t="n">
+      <c r="Q33" t="n">
         <v>90</v>
       </c>
     </row>
@@ -2944,27 +3702,33 @@
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I34" t="n">
+        <v>2.666666666666667</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="n">
         <v>1</v>
       </c>
-      <c r="J34" t="n">
-        <v>0</v>
-      </c>
-      <c r="K34" t="n">
-        <v>0</v>
-      </c>
       <c r="L34" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="n">
         <v>1</v>
       </c>
-      <c r="M34" t="n">
-        <v>0</v>
-      </c>
-      <c r="N34" t="n">
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" t="n">
         <v>6.666666666666667</v>
       </c>
-      <c r="O34" t="n">
+      <c r="Q34" t="n">
         <v>93</v>
       </c>
     </row>
@@ -2991,27 +3755,33 @@
         <v>3</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="I35" t="n">
+        <v>6</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="n">
         <v>1</v>
       </c>
-      <c r="J35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K35" t="n">
-        <v>0</v>
-      </c>
       <c r="L35" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="n">
         <v>1</v>
       </c>
-      <c r="M35" t="n">
-        <v>0</v>
-      </c>
-      <c r="N35" t="n">
+      <c r="O35" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" t="n">
         <v>17.39130434782609</v>
       </c>
-      <c r="O35" t="n">
+      <c r="Q35" t="n">
         <v>105</v>
       </c>
     </row>
@@ -3038,27 +3808,33 @@
         <v>-0.5</v>
       </c>
       <c r="H36" t="n">
+        <v>9</v>
+      </c>
+      <c r="I36" t="n">
+        <v>7</v>
+      </c>
+      <c r="J36" t="n">
         <v>5</v>
       </c>
-      <c r="I36" t="n">
+      <c r="K36" t="n">
         <v>6</v>
       </c>
-      <c r="J36" t="n">
-        <v>0</v>
-      </c>
-      <c r="K36" t="n">
-        <v>0</v>
-      </c>
       <c r="L36" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" t="n">
         <v>1</v>
       </c>
-      <c r="M36" t="n">
-        <v>0</v>
-      </c>
-      <c r="N36" t="n">
+      <c r="O36" t="n">
+        <v>0</v>
+      </c>
+      <c r="P36" t="n">
         <v>5.172413793103448</v>
       </c>
-      <c r="O36" t="n">
+      <c r="Q36" t="n">
         <v>106</v>
       </c>
     </row>
@@ -3085,27 +3861,33 @@
         <v>1.166666666666667</v>
       </c>
       <c r="H37" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="I37" t="n">
+        <v>10.33333333333333</v>
+      </c>
+      <c r="J37" t="n">
         <v>4</v>
       </c>
-      <c r="I37" t="n">
+      <c r="K37" t="n">
         <v>10</v>
       </c>
-      <c r="J37" t="n">
+      <c r="L37" t="n">
         <v>-0.2</v>
       </c>
-      <c r="K37" t="n">
-        <v>0</v>
-      </c>
-      <c r="L37" t="n">
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
         <v>1</v>
       </c>
-      <c r="M37" t="n">
-        <v>0</v>
-      </c>
-      <c r="N37" t="n">
+      <c r="O37" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" t="n">
         <v>11.50442477876106</v>
       </c>
-      <c r="O37" t="n">
+      <c r="Q37" t="n">
         <v>115</v>
       </c>
     </row>
@@ -3132,27 +3914,33 @@
         <v>-0.9230769230769231</v>
       </c>
       <c r="H38" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I38" t="n">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" t="n">
         <v>10</v>
       </c>
-      <c r="J38" t="n">
+      <c r="L38" t="n">
         <v>-1</v>
       </c>
-      <c r="K38" t="n">
-        <v>0</v>
-      </c>
-      <c r="L38" t="n">
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
         <v>1</v>
       </c>
-      <c r="M38" t="n">
-        <v>0</v>
-      </c>
-      <c r="N38" t="n">
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" t="n">
         <v>0.8333333333333334</v>
       </c>
-      <c r="O38" t="n">
+      <c r="Q38" t="n">
         <v>116</v>
       </c>
     </row>
@@ -3179,27 +3967,33 @@
         <v>8</v>
       </c>
       <c r="H39" t="n">
+        <v>5</v>
+      </c>
+      <c r="I39" t="n">
+        <v>7.666666666666667</v>
+      </c>
+      <c r="J39" t="n">
         <v>6</v>
       </c>
-      <c r="I39" t="n">
+      <c r="K39" t="n">
         <v>16</v>
       </c>
-      <c r="J39" t="n">
-        <v>0</v>
-      </c>
-      <c r="K39" t="n">
-        <v>0</v>
-      </c>
       <c r="L39" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="n">
         <v>1</v>
       </c>
-      <c r="M39" t="n">
-        <v>0</v>
-      </c>
-      <c r="N39" t="n">
+      <c r="O39" t="n">
+        <v>0</v>
+      </c>
+      <c r="P39" t="n">
         <v>3.703703703703703</v>
       </c>
-      <c r="O39" t="n">
+      <c r="Q39" t="n">
         <v>119</v>
       </c>
     </row>
@@ -3229,24 +4023,30 @@
         <v>7</v>
       </c>
       <c r="I40" t="n">
+        <v>5</v>
+      </c>
+      <c r="J40" t="n">
+        <v>7</v>
+      </c>
+      <c r="K40" t="n">
         <v>23</v>
       </c>
-      <c r="J40" t="n">
+      <c r="L40" t="n">
         <v>0.1666666666666667</v>
       </c>
-      <c r="K40" t="n">
-        <v>0</v>
-      </c>
-      <c r="L40" t="n">
+      <c r="M40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" t="n">
         <v>1</v>
       </c>
-      <c r="M40" t="n">
-        <v>0</v>
-      </c>
-      <c r="N40" t="n">
+      <c r="O40" t="n">
+        <v>0</v>
+      </c>
+      <c r="P40" t="n">
         <v>3.90625</v>
       </c>
-      <c r="O40" t="n">
+      <c r="Q40" t="n">
         <v>117</v>
       </c>
     </row>
@@ -3273,27 +4073,33 @@
         <v>0</v>
       </c>
       <c r="H41" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I41" t="n">
+        <v>6.333333333333333</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" t="n">
         <v>23</v>
       </c>
-      <c r="J41" t="n">
+      <c r="L41" t="n">
         <v>-1</v>
       </c>
-      <c r="K41" t="n">
-        <v>0</v>
-      </c>
-      <c r="L41" t="n">
+      <c r="M41" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" t="n">
         <v>1</v>
       </c>
-      <c r="M41" t="n">
-        <v>0</v>
-      </c>
-      <c r="N41" t="n">
+      <c r="O41" t="n">
+        <v>0</v>
+      </c>
+      <c r="P41" t="n">
         <v>5.376344086021505</v>
       </c>
-      <c r="O41" t="n">
+      <c r="Q41" t="n">
         <v>122</v>
       </c>
     </row>
@@ -3320,27 +4126,33 @@
         <v>3</v>
       </c>
       <c r="H42" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I42" t="n">
+        <v>10</v>
+      </c>
+      <c r="J42" t="n">
         <v>1</v>
       </c>
-      <c r="I42" t="n">
+      <c r="K42" t="n">
         <v>24</v>
       </c>
-      <c r="J42" t="n">
-        <v>0</v>
-      </c>
-      <c r="K42" t="n">
+      <c r="L42" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" t="n">
         <v>2</v>
       </c>
-      <c r="L42" t="n">
+      <c r="N42" t="n">
         <v>3</v>
       </c>
-      <c r="M42" t="n">
-        <v>0</v>
-      </c>
-      <c r="N42" t="n">
+      <c r="O42" t="n">
+        <v>0</v>
+      </c>
+      <c r="P42" t="n">
         <v>15.50387596899225</v>
       </c>
-      <c r="O42" t="n">
+      <c r="Q42" t="n">
         <v>141</v>
       </c>
     </row>
@@ -3367,27 +4179,33 @@
         <v>-0.05000000000000004</v>
       </c>
       <c r="H43" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="I43" t="n">
+        <v>14.66666666666667</v>
+      </c>
+      <c r="J43" t="n">
         <v>6</v>
       </c>
-      <c r="I43" t="n">
+      <c r="K43" t="n">
         <v>30</v>
-      </c>
-      <c r="J43" t="n">
-        <v>5</v>
-      </c>
-      <c r="K43" t="n">
-        <v>2</v>
       </c>
       <c r="L43" t="n">
         <v>5</v>
       </c>
       <c r="M43" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N43" t="n">
+        <v>5</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0</v>
+      </c>
+      <c r="P43" t="n">
         <v>7.335907335907336</v>
       </c>
-      <c r="O43" t="n">
+      <c r="Q43" t="n">
         <v>154</v>
       </c>
     </row>
@@ -3414,27 +4232,33 @@
         <v>1.105263157894737</v>
       </c>
       <c r="H44" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="I44" t="n">
+        <v>26.33333333333333</v>
+      </c>
+      <c r="J44" t="n">
         <v>7</v>
       </c>
-      <c r="I44" t="n">
+      <c r="K44" t="n">
         <v>37</v>
       </c>
-      <c r="J44" t="n">
+      <c r="L44" t="n">
         <v>0.1666666666666667</v>
       </c>
-      <c r="K44" t="n">
+      <c r="M44" t="n">
         <v>1</v>
       </c>
-      <c r="L44" t="n">
+      <c r="N44" t="n">
         <v>6</v>
       </c>
-      <c r="M44" t="n">
+      <c r="O44" t="n">
         <v>-0.5</v>
       </c>
-      <c r="N44" t="n">
+      <c r="P44" t="n">
         <v>18.34862385321101</v>
       </c>
-      <c r="O44" t="n">
+      <c r="Q44" t="n">
         <v>187</v>
       </c>
     </row>
@@ -3461,27 +4285,33 @@
         <v>-0.925</v>
       </c>
       <c r="H45" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="I45" t="n">
+        <v>20.66666666666667</v>
+      </c>
+      <c r="J45" t="n">
         <v>1</v>
       </c>
-      <c r="I45" t="n">
+      <c r="K45" t="n">
         <v>38</v>
       </c>
-      <c r="J45" t="n">
+      <c r="L45" t="n">
         <v>-0.8571428571428572</v>
       </c>
-      <c r="K45" t="n">
+      <c r="M45" t="n">
         <v>1</v>
       </c>
-      <c r="L45" t="n">
+      <c r="N45" t="n">
         <v>7</v>
       </c>
-      <c r="M45" t="n">
-        <v>0</v>
-      </c>
-      <c r="N45" t="n">
+      <c r="O45" t="n">
+        <v>0</v>
+      </c>
+      <c r="P45" t="n">
         <v>2.564102564102564</v>
       </c>
-      <c r="O45" t="n">
+      <c r="Q45" t="n">
         <v>189</v>
       </c>
     </row>
@@ -3508,27 +4338,33 @@
         <v>6.666666666666667</v>
       </c>
       <c r="H46" t="n">
+        <v>13</v>
+      </c>
+      <c r="I46" t="n">
+        <v>22</v>
+      </c>
+      <c r="J46" t="n">
         <v>14</v>
       </c>
-      <c r="I46" t="n">
+      <c r="K46" t="n">
         <v>52</v>
       </c>
-      <c r="J46" t="n">
+      <c r="L46" t="n">
         <v>13</v>
       </c>
-      <c r="K46" t="n">
-        <v>0</v>
-      </c>
-      <c r="L46" t="n">
+      <c r="M46" t="n">
+        <v>0</v>
+      </c>
+      <c r="N46" t="n">
         <v>7</v>
       </c>
-      <c r="M46" t="n">
+      <c r="O46" t="n">
         <v>-1</v>
       </c>
-      <c r="N46" t="n">
+      <c r="P46" t="n">
         <v>12.16931216931217</v>
       </c>
-      <c r="O46" t="n">
+      <c r="Q46" t="n">
         <v>198</v>
       </c>
     </row>
@@ -3555,27 +4391,33 @@
         <v>0.4347826086956521</v>
       </c>
       <c r="H47" t="n">
+        <v>28</v>
+      </c>
+      <c r="I47" t="n">
+        <v>19.66666666666667</v>
+      </c>
+      <c r="J47" t="n">
         <v>6</v>
       </c>
-      <c r="I47" t="n">
+      <c r="K47" t="n">
         <v>58</v>
       </c>
-      <c r="J47" t="n">
+      <c r="L47" t="n">
         <v>-0.5714285714285714</v>
       </c>
-      <c r="K47" t="n">
-        <v>0</v>
-      </c>
-      <c r="L47" t="n">
+      <c r="M47" t="n">
+        <v>0</v>
+      </c>
+      <c r="N47" t="n">
         <v>7</v>
       </c>
-      <c r="M47" t="n">
-        <v>0</v>
-      </c>
-      <c r="N47" t="n">
+      <c r="O47" t="n">
+        <v>0</v>
+      </c>
+      <c r="P47" t="n">
         <v>25.38461538461538</v>
       </c>
-      <c r="O47" t="n">
+      <c r="Q47" t="n">
         <v>225</v>
       </c>
     </row>
@@ -3602,27 +4444,33 @@
         <v>1.393939393939394</v>
       </c>
       <c r="H48" t="n">
+        <v>56</v>
+      </c>
+      <c r="I48" t="n">
+        <v>45</v>
+      </c>
+      <c r="J48" t="n">
         <v>1</v>
       </c>
-      <c r="I48" t="n">
+      <c r="K48" t="n">
         <v>59</v>
       </c>
-      <c r="J48" t="n">
+      <c r="L48" t="n">
         <v>-0.8333333333333334</v>
       </c>
-      <c r="K48" t="n">
-        <v>0</v>
-      </c>
-      <c r="L48" t="n">
+      <c r="M48" t="n">
+        <v>0</v>
+      </c>
+      <c r="N48" t="n">
         <v>7</v>
       </c>
-      <c r="M48" t="n">
-        <v>0</v>
-      </c>
-      <c r="N48" t="n">
+      <c r="O48" t="n">
+        <v>0</v>
+      </c>
+      <c r="P48" t="n">
         <v>31.6</v>
       </c>
-      <c r="O48" t="n">
+      <c r="Q48" t="n">
         <v>303</v>
       </c>
     </row>
@@ -3649,27 +4497,33 @@
         <v>-0.810126582278481</v>
       </c>
       <c r="H49" t="n">
+        <v>47</v>
+      </c>
+      <c r="I49" t="n">
+        <v>42.33333333333334</v>
+      </c>
+      <c r="J49" t="n">
         <v>4</v>
       </c>
-      <c r="I49" t="n">
+      <c r="K49" t="n">
         <v>63</v>
       </c>
-      <c r="J49" t="n">
+      <c r="L49" t="n">
         <v>3</v>
       </c>
-      <c r="K49" t="n">
+      <c r="M49" t="n">
         <v>1</v>
       </c>
-      <c r="L49" t="n">
+      <c r="N49" t="n">
         <v>8</v>
       </c>
-      <c r="M49" t="n">
-        <v>0</v>
-      </c>
-      <c r="N49" t="n">
+      <c r="O49" t="n">
+        <v>0</v>
+      </c>
+      <c r="P49" t="n">
         <v>9.740259740259742</v>
       </c>
-      <c r="O49" t="n">
+      <c r="Q49" t="n">
         <v>314</v>
       </c>
     </row>
@@ -3696,27 +4550,33 @@
         <v>-0.3333333333333334</v>
       </c>
       <c r="H50" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I50" t="n">
+        <v>34.66666666666666</v>
+      </c>
+      <c r="J50" t="n">
         <v>3</v>
       </c>
-      <c r="I50" t="n">
+      <c r="K50" t="n">
         <v>66</v>
       </c>
-      <c r="J50" t="n">
+      <c r="L50" t="n">
         <v>-0.25</v>
       </c>
-      <c r="K50" t="n">
-        <v>0</v>
-      </c>
-      <c r="L50" t="n">
+      <c r="M50" t="n">
+        <v>0</v>
+      </c>
+      <c r="N50" t="n">
         <v>8</v>
       </c>
-      <c r="M50" t="n">
+      <c r="O50" t="n">
         <v>-1</v>
       </c>
-      <c r="N50" t="n">
+      <c r="P50" t="n">
         <v>7.2992700729927</v>
       </c>
-      <c r="O50" t="n">
+      <c r="Q50" t="n">
         <v>321</v>
       </c>
     </row>
@@ -3743,27 +4603,33 @@
         <v>2.6</v>
       </c>
       <c r="H51" t="n">
+        <v>23</v>
+      </c>
+      <c r="I51" t="n">
+        <v>20.33333333333333</v>
+      </c>
+      <c r="J51" t="n">
         <v>5</v>
       </c>
-      <c r="I51" t="n">
+      <c r="K51" t="n">
         <v>71</v>
       </c>
-      <c r="J51" t="n">
+      <c r="L51" t="n">
         <v>0.6666666666666667</v>
       </c>
-      <c r="K51" t="n">
+      <c r="M51" t="n">
         <v>1</v>
       </c>
-      <c r="L51" t="n">
+      <c r="N51" t="n">
         <v>9</v>
       </c>
-      <c r="M51" t="n">
-        <v>0</v>
-      </c>
-      <c r="N51" t="n">
+      <c r="O51" t="n">
+        <v>0</v>
+      </c>
+      <c r="P51" t="n">
         <v>20.93023255813954</v>
       </c>
-      <c r="O51" t="n">
+      <c r="Q51" t="n">
         <v>352</v>
       </c>
     </row>
@@ -3790,27 +4656,33 @@
         <v>-0.2777777777777778</v>
       </c>
       <c r="H52" t="n">
+        <v>31</v>
+      </c>
+      <c r="I52" t="n">
+        <v>24</v>
+      </c>
+      <c r="J52" t="n">
         <v>8</v>
       </c>
-      <c r="I52" t="n">
+      <c r="K52" t="n">
         <v>79</v>
       </c>
-      <c r="J52" t="n">
+      <c r="L52" t="n">
         <v>0.6000000000000001</v>
       </c>
-      <c r="K52" t="n">
+      <c r="M52" t="n">
         <v>2</v>
       </c>
-      <c r="L52" t="n">
+      <c r="N52" t="n">
         <v>11</v>
       </c>
-      <c r="M52" t="n">
+      <c r="O52" t="n">
         <v>1</v>
       </c>
-      <c r="N52" t="n">
+      <c r="P52" t="n">
         <v>13.33333333333333</v>
       </c>
-      <c r="O52" t="n">
+      <c r="Q52" t="n">
         <v>370</v>
       </c>
     </row>
@@ -3837,27 +4709,33 @@
         <v>0.1923076923076923</v>
       </c>
       <c r="H53" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="I53" t="n">
+        <v>31</v>
+      </c>
+      <c r="J53" t="n">
         <v>5</v>
       </c>
-      <c r="I53" t="n">
+      <c r="K53" t="n">
         <v>84</v>
       </c>
-      <c r="J53" t="n">
+      <c r="L53" t="n">
         <v>-0.375</v>
       </c>
-      <c r="K53" t="n">
+      <c r="M53" t="n">
         <v>1</v>
       </c>
-      <c r="L53" t="n">
+      <c r="N53" t="n">
         <v>12</v>
       </c>
-      <c r="M53" t="n">
+      <c r="O53" t="n">
         <v>-0.5</v>
       </c>
-      <c r="N53" t="n">
+      <c r="P53" t="n">
         <v>14.83253588516746</v>
       </c>
-      <c r="O53" t="n">
+      <c r="Q53" t="n">
         <v>396</v>
       </c>
     </row>
@@ -3884,27 +4762,33 @@
         <v>-0.032258064516129</v>
       </c>
       <c r="H54" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="I54" t="n">
+        <v>29</v>
+      </c>
+      <c r="J54" t="n">
         <v>9</v>
       </c>
-      <c r="I54" t="n">
+      <c r="K54" t="n">
         <v>93</v>
       </c>
-      <c r="J54" t="n">
+      <c r="L54" t="n">
         <v>0.8</v>
       </c>
-      <c r="K54" t="n">
-        <v>0</v>
-      </c>
-      <c r="L54" t="n">
+      <c r="M54" t="n">
+        <v>0</v>
+      </c>
+      <c r="N54" t="n">
         <v>12</v>
       </c>
-      <c r="M54" t="n">
+      <c r="O54" t="n">
         <v>-1</v>
       </c>
-      <c r="N54" t="n">
+      <c r="P54" t="n">
         <v>12.39669421487603</v>
       </c>
-      <c r="O54" t="n">
+      <c r="Q54" t="n">
         <v>417</v>
       </c>
     </row>
@@ -3931,27 +4815,33 @@
         <v>0.7</v>
       </c>
       <c r="H55" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="I55" t="n">
+        <v>37.33333333333334</v>
+      </c>
+      <c r="J55" t="n">
         <v>9</v>
       </c>
-      <c r="I55" t="n">
+      <c r="K55" t="n">
         <v>102</v>
       </c>
-      <c r="J55" t="n">
-        <v>0</v>
-      </c>
-      <c r="K55" t="n">
-        <v>0</v>
-      </c>
       <c r="L55" t="n">
+        <v>0</v>
+      </c>
+      <c r="M55" t="n">
+        <v>0</v>
+      </c>
+      <c r="N55" t="n">
         <v>12</v>
       </c>
-      <c r="M55" t="n">
-        <v>0</v>
-      </c>
-      <c r="N55" t="n">
+      <c r="O55" t="n">
+        <v>0</v>
+      </c>
+      <c r="P55" t="n">
         <v>17.3469387755102</v>
       </c>
-      <c r="O55" t="n">
+      <c r="Q55" t="n">
         <v>459</v>
       </c>
     </row>
@@ -3978,27 +4868,33 @@
         <v>-0.2745098039215687</v>
       </c>
       <c r="H56" t="n">
+        <v>44</v>
+      </c>
+      <c r="I56" t="n">
+        <v>39.33333333333334</v>
+      </c>
+      <c r="J56" t="n">
         <v>21</v>
       </c>
-      <c r="I56" t="n">
+      <c r="K56" t="n">
         <v>123</v>
       </c>
-      <c r="J56" t="n">
+      <c r="L56" t="n">
         <v>1.333333333333333</v>
       </c>
-      <c r="K56" t="n">
+      <c r="M56" t="n">
         <v>3</v>
       </c>
-      <c r="L56" t="n">
+      <c r="N56" t="n">
         <v>15</v>
       </c>
-      <c r="M56" t="n">
-        <v>0</v>
-      </c>
-      <c r="N56" t="n">
+      <c r="O56" t="n">
+        <v>0</v>
+      </c>
+      <c r="P56" t="n">
         <v>10.48158640226629</v>
       </c>
-      <c r="O56" t="n">
+      <c r="Q56" t="n">
         <v>475</v>
       </c>
     </row>
@@ -4025,27 +4921,33 @@
         <v>-0.8378378378378378</v>
       </c>
       <c r="H57" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="I57" t="n">
+        <v>31.33333333333333</v>
+      </c>
+      <c r="J57" t="n">
         <v>5</v>
       </c>
-      <c r="I57" t="n">
+      <c r="K57" t="n">
         <v>128</v>
       </c>
-      <c r="J57" t="n">
+      <c r="L57" t="n">
         <v>-0.7619047619047619</v>
       </c>
-      <c r="K57" t="n">
-        <v>0</v>
-      </c>
-      <c r="L57" t="n">
+      <c r="M57" t="n">
+        <v>0</v>
+      </c>
+      <c r="N57" t="n">
         <v>15</v>
       </c>
-      <c r="M57" t="n">
+      <c r="O57" t="n">
         <v>-1</v>
       </c>
-      <c r="N57" t="n">
+      <c r="P57" t="n">
         <v>3.141361256544502</v>
       </c>
-      <c r="O57" t="n">
+      <c r="Q57" t="n">
         <v>476</v>
       </c>
     </row>
@@ -4072,27 +4974,33 @@
         <v>3.333333333333333</v>
       </c>
       <c r="H58" t="n">
+        <v>16</v>
+      </c>
+      <c r="I58" t="n">
+        <v>23</v>
+      </c>
+      <c r="J58" t="n">
         <v>10</v>
       </c>
-      <c r="I58" t="n">
+      <c r="K58" t="n">
         <v>138</v>
       </c>
-      <c r="J58" t="n">
+      <c r="L58" t="n">
         <v>1</v>
       </c>
-      <c r="K58" t="n">
+      <c r="M58" t="n">
         <v>3</v>
       </c>
-      <c r="L58" t="n">
+      <c r="N58" t="n">
         <v>18</v>
       </c>
-      <c r="M58" t="n">
-        <v>0</v>
-      </c>
-      <c r="N58" t="n">
+      <c r="O58" t="n">
+        <v>0</v>
+      </c>
+      <c r="P58" t="n">
         <v>15.11627906976744</v>
       </c>
-      <c r="O58" t="n">
+      <c r="Q58" t="n">
         <v>492</v>
       </c>
     </row>
@@ -4119,27 +5027,33 @@
         <v>0.5</v>
       </c>
       <c r="H59" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="I59" t="n">
+        <v>23.66666666666667</v>
+      </c>
+      <c r="J59" t="n">
         <v>21</v>
       </c>
-      <c r="I59" t="n">
+      <c r="K59" t="n">
         <v>159</v>
       </c>
-      <c r="J59" t="n">
+      <c r="L59" t="n">
         <v>1.1</v>
       </c>
-      <c r="K59" t="n">
+      <c r="M59" t="n">
         <v>1</v>
       </c>
-      <c r="L59" t="n">
+      <c r="N59" t="n">
         <v>19</v>
       </c>
-      <c r="M59" t="n">
+      <c r="O59" t="n">
         <v>-0.6666666666666667</v>
       </c>
-      <c r="N59" t="n">
+      <c r="P59" t="n">
         <v>15.29411764705882</v>
       </c>
-      <c r="O59" t="n">
+      <c r="Q59" t="n">
         <v>510</v>
       </c>
     </row>
@@ -4166,27 +5080,33 @@
         <v>-0.1282051282051282</v>
       </c>
       <c r="H60" t="n">
+        <v>36.5</v>
+      </c>
+      <c r="I60" t="n">
+        <v>33</v>
+      </c>
+      <c r="J60" t="n">
         <v>3</v>
       </c>
-      <c r="I60" t="n">
+      <c r="K60" t="n">
         <v>162</v>
       </c>
-      <c r="J60" t="n">
+      <c r="L60" t="n">
         <v>-0.8571428571428572</v>
       </c>
-      <c r="K60" t="n">
-        <v>0</v>
-      </c>
-      <c r="L60" t="n">
+      <c r="M60" t="n">
+        <v>0</v>
+      </c>
+      <c r="N60" t="n">
         <v>19</v>
       </c>
-      <c r="M60" t="n">
+      <c r="O60" t="n">
         <v>-1</v>
       </c>
-      <c r="N60" t="n">
+      <c r="P60" t="n">
         <v>12.92775665399239</v>
       </c>
-      <c r="O60" t="n">
+      <c r="Q60" t="n">
         <v>541</v>
       </c>
     </row>
@@ -4213,27 +5133,33 @@
         <v>-0.1764705882352942</v>
       </c>
       <c r="H61" t="n">
+        <v>31</v>
+      </c>
+      <c r="I61" t="n">
+        <v>33.66666666666666</v>
+      </c>
+      <c r="J61" t="n">
         <v>3</v>
       </c>
-      <c r="I61" t="n">
+      <c r="K61" t="n">
         <v>165</v>
       </c>
-      <c r="J61" t="n">
-        <v>0</v>
-      </c>
-      <c r="K61" t="n">
+      <c r="L61" t="n">
+        <v>0</v>
+      </c>
+      <c r="M61" t="n">
         <v>1</v>
       </c>
-      <c r="L61" t="n">
+      <c r="N61" t="n">
         <v>20</v>
       </c>
-      <c r="M61" t="n">
-        <v>0</v>
-      </c>
-      <c r="N61" t="n">
+      <c r="O61" t="n">
+        <v>0</v>
+      </c>
+      <c r="P61" t="n">
         <v>9.621993127147768</v>
       </c>
-      <c r="O61" t="n">
+      <c r="Q61" t="n">
         <v>566</v>
       </c>
     </row>
@@ -4260,27 +5186,33 @@
         <v>0.1428571428571428</v>
       </c>
       <c r="H62" t="n">
+        <v>30</v>
+      </c>
+      <c r="I62" t="n">
+        <v>31.33333333333333</v>
+      </c>
+      <c r="J62" t="n">
         <v>1</v>
       </c>
-      <c r="I62" t="n">
+      <c r="K62" t="n">
         <v>166</v>
       </c>
-      <c r="J62" t="n">
+      <c r="L62" t="n">
         <v>-0.6666666666666667</v>
       </c>
-      <c r="K62" t="n">
+      <c r="M62" t="n">
         <v>1</v>
       </c>
-      <c r="L62" t="n">
+      <c r="N62" t="n">
         <v>21</v>
       </c>
-      <c r="M62" t="n">
-        <v>0</v>
-      </c>
-      <c r="N62" t="n">
+      <c r="O62" t="n">
+        <v>0</v>
+      </c>
+      <c r="P62" t="n">
         <v>10.77441077441077</v>
       </c>
-      <c r="O62" t="n">
+      <c r="Q62" t="n">
         <v>597</v>
       </c>
     </row>
@@ -4307,27 +5239,33 @@
         <v>-0.46875</v>
       </c>
       <c r="H63" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="I63" t="n">
+        <v>25.66666666666667</v>
+      </c>
+      <c r="J63" t="n">
         <v>35</v>
       </c>
-      <c r="I63" t="n">
+      <c r="K63" t="n">
         <v>201</v>
       </c>
-      <c r="J63" t="n">
+      <c r="L63" t="n">
         <v>34</v>
       </c>
-      <c r="K63" t="n">
+      <c r="M63" t="n">
         <v>1</v>
       </c>
-      <c r="L63" t="n">
+      <c r="N63" t="n">
         <v>22</v>
       </c>
-      <c r="M63" t="n">
-        <v>0</v>
-      </c>
-      <c r="N63" t="n">
+      <c r="O63" t="n">
+        <v>0</v>
+      </c>
+      <c r="P63" t="n">
         <v>7.555555555555555</v>
       </c>
-      <c r="O63" t="n">
+      <c r="Q63" t="n">
         <v>579</v>
       </c>
     </row>
@@ -4354,27 +5292,33 @@
         <v>-0.4117647058823529</v>
       </c>
       <c r="H64" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="I64" t="n">
+        <v>19.66666666666667</v>
+      </c>
+      <c r="J64" t="n">
         <v>31</v>
       </c>
-      <c r="I64" t="n">
+      <c r="K64" t="n">
         <v>232</v>
       </c>
-      <c r="J64" t="n">
+      <c r="L64" t="n">
         <v>-0.1142857142857143</v>
       </c>
-      <c r="K64" t="n">
-        <v>0</v>
-      </c>
-      <c r="L64" t="n">
+      <c r="M64" t="n">
+        <v>0</v>
+      </c>
+      <c r="N64" t="n">
         <v>22</v>
       </c>
-      <c r="M64" t="n">
+      <c r="O64" t="n">
         <v>-1</v>
       </c>
-      <c r="N64" t="n">
+      <c r="P64" t="n">
         <v>4</v>
       </c>
-      <c r="O64" t="n">
+      <c r="Q64" t="n">
         <v>558</v>
       </c>
     </row>
@@ -4401,27 +5345,33 @@
         <v>-0.09999999999999998</v>
       </c>
       <c r="H65" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="I65" t="n">
+        <v>12</v>
+      </c>
+      <c r="J65" t="n">
         <v>17</v>
       </c>
-      <c r="I65" t="n">
+      <c r="K65" t="n">
         <v>249</v>
       </c>
-      <c r="J65" t="n">
+      <c r="L65" t="n">
         <v>-0.4516129032258065</v>
       </c>
-      <c r="K65" t="n">
-        <v>0</v>
-      </c>
-      <c r="L65" t="n">
+      <c r="M65" t="n">
+        <v>0</v>
+      </c>
+      <c r="N65" t="n">
         <v>22</v>
       </c>
-      <c r="M65" t="n">
-        <v>0</v>
-      </c>
-      <c r="N65" t="n">
+      <c r="O65" t="n">
+        <v>0</v>
+      </c>
+      <c r="P65" t="n">
         <v>4</v>
       </c>
-      <c r="O65" t="n">
+      <c r="Q65" t="n">
         <v>550</v>
       </c>
     </row>
@@ -4448,27 +5398,33 @@
         <v>-0.2222222222222222</v>
       </c>
       <c r="H66" t="n">
+        <v>8</v>
+      </c>
+      <c r="I66" t="n">
+        <v>8.666666666666666</v>
+      </c>
+      <c r="J66" t="n">
         <v>22</v>
       </c>
-      <c r="I66" t="n">
+      <c r="K66" t="n">
         <v>271</v>
       </c>
-      <c r="J66" t="n">
+      <c r="L66" t="n">
         <v>0.2941176470588236</v>
       </c>
-      <c r="K66" t="n">
-        <v>0</v>
-      </c>
-      <c r="L66" t="n">
+      <c r="M66" t="n">
+        <v>0</v>
+      </c>
+      <c r="N66" t="n">
         <v>22</v>
       </c>
-      <c r="M66" t="n">
-        <v>0</v>
-      </c>
-      <c r="N66" t="n">
+      <c r="O66" t="n">
+        <v>0</v>
+      </c>
+      <c r="P66" t="n">
         <v>2.892561983471075</v>
       </c>
-      <c r="O66" t="n">
+      <c r="Q66" t="n">
         <v>535</v>
       </c>
     </row>
@@ -4495,27 +5451,33 @@
         <v>0</v>
       </c>
       <c r="H67" t="n">
+        <v>7</v>
+      </c>
+      <c r="I67" t="n">
+        <v>7.666666666666667</v>
+      </c>
+      <c r="J67" t="n">
         <v>27</v>
       </c>
-      <c r="I67" t="n">
+      <c r="K67" t="n">
         <v>298</v>
       </c>
-      <c r="J67" t="n">
+      <c r="L67" t="n">
         <v>0.2272727272727273</v>
       </c>
-      <c r="K67" t="n">
-        <v>0</v>
-      </c>
-      <c r="L67" t="n">
+      <c r="M67" t="n">
+        <v>0</v>
+      </c>
+      <c r="N67" t="n">
         <v>22</v>
       </c>
-      <c r="M67" t="n">
-        <v>0</v>
-      </c>
-      <c r="N67" t="n">
+      <c r="O67" t="n">
+        <v>0</v>
+      </c>
+      <c r="P67" t="n">
         <v>3.167420814479638</v>
       </c>
-      <c r="O67" t="n">
+      <c r="Q67" t="n">
         <v>515</v>
       </c>
     </row>
@@ -4542,27 +5504,33 @@
         <v>0.4285714285714286</v>
       </c>
       <c r="H68" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="I68" t="n">
+        <v>8</v>
+      </c>
+      <c r="J68" t="n">
         <v>38</v>
       </c>
-      <c r="I68" t="n">
+      <c r="K68" t="n">
         <v>336</v>
       </c>
-      <c r="J68" t="n">
+      <c r="L68" t="n">
         <v>0.4074074074074074</v>
       </c>
-      <c r="K68" t="n">
-        <v>0</v>
-      </c>
-      <c r="L68" t="n">
+      <c r="M68" t="n">
+        <v>0</v>
+      </c>
+      <c r="N68" t="n">
         <v>22</v>
       </c>
-      <c r="M68" t="n">
-        <v>0</v>
-      </c>
-      <c r="N68" t="n">
+      <c r="O68" t="n">
+        <v>0</v>
+      </c>
+      <c r="P68" t="n">
         <v>4.347826086956522</v>
       </c>
-      <c r="O68" t="n">
+      <c r="Q68" t="n">
         <v>487</v>
       </c>
     </row>
@@ -4589,27 +5557,33 @@
         <v>1.8</v>
       </c>
       <c r="H69" t="n">
+        <v>19</v>
+      </c>
+      <c r="I69" t="n">
+        <v>15</v>
+      </c>
+      <c r="J69" t="n">
         <v>45</v>
       </c>
-      <c r="I69" t="n">
+      <c r="K69" t="n">
         <v>381</v>
       </c>
-      <c r="J69" t="n">
+      <c r="L69" t="n">
         <v>0.1842105263157894</v>
       </c>
-      <c r="K69" t="n">
+      <c r="M69" t="n">
         <v>3</v>
       </c>
-      <c r="L69" t="n">
+      <c r="N69" t="n">
         <v>25</v>
       </c>
-      <c r="M69" t="n">
-        <v>0</v>
-      </c>
-      <c r="N69" t="n">
+      <c r="O69" t="n">
+        <v>0</v>
+      </c>
+      <c r="P69" t="n">
         <v>6.796116504854369</v>
       </c>
-      <c r="O69" t="n">
+      <c r="Q69" t="n">
         <v>470</v>
       </c>
     </row>
@@ -4636,27 +5610,33 @@
         <v>-0.8571428571428572</v>
       </c>
       <c r="H70" t="n">
+        <v>16</v>
+      </c>
+      <c r="I70" t="n">
+        <v>14</v>
+      </c>
+      <c r="J70" t="n">
         <v>22</v>
       </c>
-      <c r="I70" t="n">
+      <c r="K70" t="n">
         <v>403</v>
       </c>
-      <c r="J70" t="n">
+      <c r="L70" t="n">
         <v>-0.5111111111111111</v>
       </c>
-      <c r="K70" t="n">
+      <c r="M70" t="n">
         <v>1</v>
       </c>
-      <c r="L70" t="n">
+      <c r="N70" t="n">
         <v>26</v>
       </c>
-      <c r="M70" t="n">
+      <c r="O70" t="n">
         <v>-0.6666666666666667</v>
       </c>
-      <c r="N70" t="n">
+      <c r="P70" t="n">
         <v>1.574803149606299</v>
       </c>
-      <c r="O70" t="n">
+      <c r="Q70" t="n">
         <v>452</v>
       </c>
     </row>
@@ -4683,27 +5663,33 @@
         <v>-0.75</v>
       </c>
       <c r="H71" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="I71" t="n">
+        <v>11</v>
+      </c>
+      <c r="J71" t="n">
         <v>87</v>
       </c>
-      <c r="I71" t="n">
+      <c r="K71" t="n">
         <v>490</v>
       </c>
-      <c r="J71" t="n">
+      <c r="L71" t="n">
         <v>2.954545454545455</v>
       </c>
-      <c r="K71" t="n">
-        <v>0</v>
-      </c>
-      <c r="L71" t="n">
+      <c r="M71" t="n">
+        <v>0</v>
+      </c>
+      <c r="N71" t="n">
         <v>26</v>
       </c>
-      <c r="M71" t="n">
+      <c r="O71" t="n">
         <v>-1</v>
       </c>
-      <c r="N71" t="n">
+      <c r="P71" t="n">
         <v>0.4545454545454545</v>
       </c>
-      <c r="O71" t="n">
+      <c r="Q71" t="n">
         <v>366</v>
       </c>
     </row>
@@ -4730,27 +5716,33 @@
         <v>3</v>
       </c>
       <c r="H72" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="I72" t="n">
+        <v>3</v>
+      </c>
+      <c r="J72" t="n">
         <v>43</v>
       </c>
-      <c r="I72" t="n">
+      <c r="K72" t="n">
         <v>533</v>
       </c>
-      <c r="J72" t="n">
+      <c r="L72" t="n">
         <v>-0.5057471264367817</v>
       </c>
-      <c r="K72" t="n">
-        <v>0</v>
-      </c>
-      <c r="L72" t="n">
+      <c r="M72" t="n">
+        <v>0</v>
+      </c>
+      <c r="N72" t="n">
         <v>26</v>
       </c>
-      <c r="M72" t="n">
-        <v>0</v>
-      </c>
-      <c r="N72" t="n">
+      <c r="O72" t="n">
+        <v>0</v>
+      </c>
+      <c r="P72" t="n">
         <v>1.234567901234568</v>
       </c>
-      <c r="O72" t="n">
+      <c r="Q72" t="n">
         <v>327</v>
       </c>
     </row>
@@ -4777,27 +5769,33 @@
         <v>-0.75</v>
       </c>
       <c r="H73" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="I73" t="n">
+        <v>2</v>
+      </c>
+      <c r="J73" t="n">
         <v>28</v>
       </c>
-      <c r="I73" t="n">
+      <c r="K73" t="n">
         <v>561</v>
       </c>
-      <c r="J73" t="n">
+      <c r="L73" t="n">
         <v>-0.3488372093023255</v>
       </c>
-      <c r="K73" t="n">
+      <c r="M73" t="n">
         <v>1</v>
       </c>
-      <c r="L73" t="n">
+      <c r="N73" t="n">
         <v>27</v>
       </c>
-      <c r="M73" t="n">
-        <v>0</v>
-      </c>
-      <c r="N73" t="n">
+      <c r="O73" t="n">
+        <v>0</v>
+      </c>
+      <c r="P73" t="n">
         <v>0.4366812227074235</v>
       </c>
-      <c r="O73" t="n">
+      <c r="Q73" t="n">
         <v>300</v>
       </c>
     </row>
@@ -4824,27 +5822,33 @@
         <v>0</v>
       </c>
       <c r="H74" t="n">
+        <v>1</v>
+      </c>
+      <c r="I74" t="n">
+        <v>2</v>
+      </c>
+      <c r="J74" t="n">
         <v>61</v>
       </c>
-      <c r="I74" t="n">
+      <c r="K74" t="n">
         <v>622</v>
       </c>
-      <c r="J74" t="n">
+      <c r="L74" t="n">
         <v>1.178571428571428</v>
       </c>
-      <c r="K74" t="n">
+      <c r="M74" t="n">
         <v>1</v>
       </c>
-      <c r="L74" t="n">
+      <c r="N74" t="n">
         <v>28</v>
       </c>
-      <c r="M74" t="n">
-        <v>0</v>
-      </c>
-      <c r="N74" t="n">
+      <c r="O74" t="n">
+        <v>0</v>
+      </c>
+      <c r="P74" t="n">
         <v>0.411522633744856</v>
       </c>
-      <c r="O74" t="n">
+      <c r="Q74" t="n">
         <v>240</v>
       </c>
     </row>
@@ -4871,27 +5875,33 @@
         <v>7</v>
       </c>
       <c r="H75" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="I75" t="n">
+        <v>3.333333333333333</v>
+      </c>
+      <c r="J75" t="n">
         <v>31</v>
       </c>
-      <c r="I75" t="n">
+      <c r="K75" t="n">
         <v>653</v>
       </c>
-      <c r="J75" t="n">
+      <c r="L75" t="n">
         <v>-0.4918032786885246</v>
       </c>
-      <c r="K75" t="n">
-        <v>0</v>
-      </c>
-      <c r="L75" t="n">
+      <c r="M75" t="n">
+        <v>0</v>
+      </c>
+      <c r="N75" t="n">
         <v>28</v>
       </c>
-      <c r="M75" t="n">
+      <c r="O75" t="n">
         <v>-1</v>
       </c>
-      <c r="N75" t="n">
+      <c r="P75" t="n">
         <v>4.519774011299435</v>
       </c>
-      <c r="O75" t="n">
+      <c r="Q75" t="n">
         <v>217</v>
       </c>
     </row>
@@ -4918,27 +5928,33 @@
         <v>0.75</v>
       </c>
       <c r="H76" t="n">
+        <v>11</v>
+      </c>
+      <c r="I76" t="n">
+        <v>7.666666666666667</v>
+      </c>
+      <c r="J76" t="n">
         <v>2</v>
       </c>
-      <c r="I76" t="n">
+      <c r="K76" t="n">
         <v>655</v>
       </c>
-      <c r="J76" t="n">
+      <c r="L76" t="n">
         <v>-0.935483870967742</v>
       </c>
-      <c r="K76" t="n">
-        <v>0</v>
-      </c>
-      <c r="L76" t="n">
+      <c r="M76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N76" t="n">
         <v>28</v>
       </c>
-      <c r="M76" t="n">
-        <v>0</v>
-      </c>
-      <c r="N76" t="n">
+      <c r="O76" t="n">
+        <v>0</v>
+      </c>
+      <c r="P76" t="n">
         <v>7.000000000000001</v>
       </c>
-      <c r="O76" t="n">
+      <c r="Q76" t="n">
         <v>229</v>
       </c>
     </row>
@@ -4965,27 +5981,33 @@
         <v>-0.2142857142857143</v>
       </c>
       <c r="H77" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I77" t="n">
+        <v>11</v>
+      </c>
+      <c r="J77" t="n">
         <v>2</v>
       </c>
-      <c r="I77" t="n">
+      <c r="K77" t="n">
         <v>657</v>
       </c>
-      <c r="J77" t="n">
-        <v>0</v>
-      </c>
-      <c r="K77" t="n">
-        <v>0</v>
-      </c>
       <c r="L77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M77" t="n">
+        <v>0</v>
+      </c>
+      <c r="N77" t="n">
         <v>28</v>
       </c>
-      <c r="M77" t="n">
-        <v>0</v>
-      </c>
-      <c r="N77" t="n">
+      <c r="O77" t="n">
+        <v>0</v>
+      </c>
+      <c r="P77" t="n">
         <v>5.583756345177665</v>
       </c>
-      <c r="O77" t="n">
+      <c r="Q77" t="n">
         <v>238</v>
       </c>
     </row>
@@ -5012,27 +6034,33 @@
         <v>1.181818181818182</v>
       </c>
       <c r="H78" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="I78" t="n">
+        <v>16.33333333333333</v>
+      </c>
+      <c r="J78" t="n">
         <v>14</v>
       </c>
-      <c r="I78" t="n">
+      <c r="K78" t="n">
         <v>671</v>
       </c>
-      <c r="J78" t="n">
+      <c r="L78" t="n">
         <v>6</v>
       </c>
-      <c r="K78" t="n">
+      <c r="M78" t="n">
         <v>1</v>
       </c>
-      <c r="L78" t="n">
+      <c r="N78" t="n">
         <v>29</v>
       </c>
-      <c r="M78" t="n">
-        <v>0</v>
-      </c>
-      <c r="N78" t="n">
+      <c r="O78" t="n">
+        <v>0</v>
+      </c>
+      <c r="P78" t="n">
         <v>9.338521400778211</v>
       </c>
-      <c r="O78" t="n">
+      <c r="Q78" t="n">
         <v>248</v>
       </c>
     </row>
@@ -5059,27 +6087,33 @@
         <v>-0.6666666666666667</v>
       </c>
       <c r="H79" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I79" t="n">
+        <v>14.33333333333333</v>
+      </c>
+      <c r="J79" t="n">
+        <v>0</v>
+      </c>
+      <c r="K79" t="n">
         <v>671</v>
       </c>
-      <c r="J79" t="n">
+      <c r="L79" t="n">
         <v>-1</v>
       </c>
-      <c r="K79" t="n">
-        <v>0</v>
-      </c>
-      <c r="L79" t="n">
+      <c r="M79" t="n">
+        <v>0</v>
+      </c>
+      <c r="N79" t="n">
         <v>29</v>
       </c>
-      <c r="M79" t="n">
+      <c r="O79" t="n">
         <v>-1</v>
       </c>
-      <c r="N79" t="n">
+      <c r="P79" t="n">
         <v>3.137254901960784</v>
       </c>
-      <c r="O79" t="n">
+      <c r="Q79" t="n">
         <v>256</v>
       </c>
     </row>
@@ -5106,27 +6140,33 @@
         <v>1.25</v>
       </c>
       <c r="H80" t="n">
+        <v>13</v>
+      </c>
+      <c r="I80" t="n">
+        <v>16.66666666666667</v>
+      </c>
+      <c r="J80" t="n">
         <v>19</v>
       </c>
-      <c r="I80" t="n">
+      <c r="K80" t="n">
         <v>690</v>
       </c>
-      <c r="J80" t="n">
-        <v>0</v>
-      </c>
-      <c r="K80" t="n">
-        <v>0</v>
-      </c>
       <c r="L80" t="n">
+        <v>0</v>
+      </c>
+      <c r="M80" t="n">
+        <v>0</v>
+      </c>
+      <c r="N80" t="n">
         <v>29</v>
       </c>
-      <c r="M80" t="n">
-        <v>0</v>
-      </c>
-      <c r="N80" t="n">
+      <c r="O80" t="n">
+        <v>0</v>
+      </c>
+      <c r="P80" t="n">
         <v>6</v>
       </c>
-      <c r="O80" t="n">
+      <c r="Q80" t="n">
         <v>255</v>
       </c>
     </row>
@@ -5153,27 +6193,33 @@
         <v>-0.4444444444444444</v>
       </c>
       <c r="H81" t="n">
+        <v>14</v>
+      </c>
+      <c r="I81" t="n">
+        <v>12</v>
+      </c>
+      <c r="J81" t="n">
         <v>1</v>
       </c>
-      <c r="I81" t="n">
+      <c r="K81" t="n">
         <v>691</v>
       </c>
-      <c r="J81" t="n">
+      <c r="L81" t="n">
         <v>-0.9473684210526316</v>
       </c>
-      <c r="K81" t="n">
-        <v>0</v>
-      </c>
-      <c r="L81" t="n">
+      <c r="M81" t="n">
+        <v>0</v>
+      </c>
+      <c r="N81" t="n">
         <v>29</v>
       </c>
-      <c r="M81" t="n">
-        <v>0</v>
-      </c>
-      <c r="N81" t="n">
+      <c r="O81" t="n">
+        <v>0</v>
+      </c>
+      <c r="P81" t="n">
         <v>4.23728813559322</v>
       </c>
-      <c r="O81" t="n">
+      <c r="Q81" t="n">
         <v>264</v>
       </c>
     </row>
@@ -5200,27 +6246,33 @@
         <v>1.3</v>
       </c>
       <c r="H82" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="I82" t="n">
+        <v>17</v>
+      </c>
+      <c r="J82" t="n">
         <v>22</v>
       </c>
-      <c r="I82" t="n">
+      <c r="K82" t="n">
         <v>713</v>
       </c>
-      <c r="J82" t="n">
+      <c r="L82" t="n">
         <v>21</v>
       </c>
-      <c r="K82" t="n">
-        <v>0</v>
-      </c>
-      <c r="L82" t="n">
+      <c r="M82" t="n">
+        <v>0</v>
+      </c>
+      <c r="N82" t="n">
         <v>29</v>
       </c>
-      <c r="M82" t="n">
-        <v>0</v>
-      </c>
-      <c r="N82" t="n">
+      <c r="O82" t="n">
+        <v>0</v>
+      </c>
+      <c r="P82" t="n">
         <v>5.651105651105651</v>
       </c>
-      <c r="O82" t="n">
+      <c r="Q82" t="n">
         <v>265</v>
       </c>
     </row>
@@ -5247,27 +6299,33 @@
         <v>-0.6956521739130435</v>
       </c>
       <c r="H83" t="n">
+        <v>15</v>
+      </c>
+      <c r="I83" t="n">
+        <v>13.33333333333333</v>
+      </c>
+      <c r="J83" t="n">
         <v>23</v>
       </c>
-      <c r="I83" t="n">
+      <c r="K83" t="n">
         <v>736</v>
       </c>
-      <c r="J83" t="n">
+      <c r="L83" t="n">
         <v>0.04545454545454541</v>
       </c>
-      <c r="K83" t="n">
-        <v>0</v>
-      </c>
-      <c r="L83" t="n">
+      <c r="M83" t="n">
+        <v>0</v>
+      </c>
+      <c r="N83" t="n">
         <v>29</v>
       </c>
-      <c r="M83" t="n">
-        <v>0</v>
-      </c>
-      <c r="N83" t="n">
+      <c r="O83" t="n">
+        <v>0</v>
+      </c>
+      <c r="P83" t="n">
         <v>3.465346534653466</v>
       </c>
-      <c r="O83" t="n">
+      <c r="Q83" t="n">
         <v>249</v>
       </c>
     </row>
@@ -5294,27 +6352,33 @@
         <v>-0.5714285714285714</v>
       </c>
       <c r="H84" t="n">
+        <v>5</v>
+      </c>
+      <c r="I84" t="n">
+        <v>11</v>
+      </c>
+      <c r="J84" t="n">
         <v>18</v>
       </c>
-      <c r="I84" t="n">
+      <c r="K84" t="n">
         <v>754</v>
       </c>
-      <c r="J84" t="n">
+      <c r="L84" t="n">
         <v>-0.2173913043478261</v>
       </c>
-      <c r="K84" t="n">
-        <v>0</v>
-      </c>
-      <c r="L84" t="n">
+      <c r="M84" t="n">
+        <v>0</v>
+      </c>
+      <c r="N84" t="n">
         <v>29</v>
       </c>
-      <c r="M84" t="n">
-        <v>0</v>
-      </c>
-      <c r="N84" t="n">
+      <c r="O84" t="n">
+        <v>0</v>
+      </c>
+      <c r="P84" t="n">
         <v>1.5</v>
       </c>
-      <c r="O84" t="n">
+      <c r="Q84" t="n">
         <v>234</v>
       </c>
     </row>
@@ -5341,27 +6405,33 @@
         <v>-0.6666666666666667</v>
       </c>
       <c r="H85" t="n">
+        <v>2</v>
+      </c>
+      <c r="I85" t="n">
+        <v>3.666666666666667</v>
+      </c>
+      <c r="J85" t="n">
         <v>15</v>
       </c>
-      <c r="I85" t="n">
+      <c r="K85" t="n">
         <v>769</v>
       </c>
-      <c r="J85" t="n">
+      <c r="L85" t="n">
         <v>-0.1666666666666666</v>
       </c>
-      <c r="K85" t="n">
-        <v>0</v>
-      </c>
-      <c r="L85" t="n">
+      <c r="M85" t="n">
+        <v>0</v>
+      </c>
+      <c r="N85" t="n">
         <v>29</v>
       </c>
-      <c r="M85" t="n">
-        <v>0</v>
-      </c>
-      <c r="N85" t="n">
+      <c r="O85" t="n">
+        <v>0</v>
+      </c>
+      <c r="P85" t="n">
         <v>0.4739336492890995</v>
       </c>
-      <c r="O85" t="n">
+      <c r="Q85" t="n">
         <v>220</v>
       </c>
     </row>
@@ -5388,27 +6458,33 @@
         <v>13</v>
       </c>
       <c r="H86" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="I86" t="n">
+        <v>6</v>
+      </c>
+      <c r="J86" t="n">
         <v>3</v>
       </c>
-      <c r="I86" t="n">
+      <c r="K86" t="n">
         <v>772</v>
       </c>
-      <c r="J86" t="n">
+      <c r="L86" t="n">
         <v>-0.8</v>
       </c>
-      <c r="K86" t="n">
-        <v>0</v>
-      </c>
-      <c r="L86" t="n">
+      <c r="M86" t="n">
+        <v>0</v>
+      </c>
+      <c r="N86" t="n">
         <v>29</v>
       </c>
-      <c r="M86" t="n">
-        <v>0</v>
-      </c>
-      <c r="N86" t="n">
+      <c r="O86" t="n">
+        <v>0</v>
+      </c>
+      <c r="P86" t="n">
         <v>6.730769230769231</v>
       </c>
-      <c r="O86" t="n">
+      <c r="Q86" t="n">
         <v>231</v>
       </c>
     </row>
@@ -5435,27 +6511,33 @@
         <v>-0.9285714285714286</v>
       </c>
       <c r="H87" t="n">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="I87" t="n">
+        <v>5.333333333333333</v>
+      </c>
+      <c r="J87" t="n">
+        <v>0</v>
+      </c>
+      <c r="K87" t="n">
         <v>772</v>
       </c>
-      <c r="J87" t="n">
+      <c r="L87" t="n">
         <v>-1</v>
       </c>
-      <c r="K87" t="n">
-        <v>0</v>
-      </c>
-      <c r="L87" t="n">
+      <c r="M87" t="n">
+        <v>0</v>
+      </c>
+      <c r="N87" t="n">
         <v>29</v>
       </c>
-      <c r="M87" t="n">
-        <v>0</v>
-      </c>
-      <c r="N87" t="n">
+      <c r="O87" t="n">
+        <v>0</v>
+      </c>
+      <c r="P87" t="n">
         <v>0.6896551724137931</v>
       </c>
-      <c r="O87" t="n">
+      <c r="Q87" t="n">
         <v>232</v>
       </c>
     </row>
@@ -5482,27 +6564,33 @@
         <v>20</v>
       </c>
       <c r="H88" t="n">
+        <v>11</v>
+      </c>
+      <c r="I88" t="n">
+        <v>12</v>
+      </c>
+      <c r="J88" t="n">
         <v>10</v>
       </c>
-      <c r="I88" t="n">
+      <c r="K88" t="n">
         <v>782</v>
       </c>
-      <c r="J88" t="n">
-        <v>0</v>
-      </c>
-      <c r="K88" t="n">
-        <v>0</v>
-      </c>
       <c r="L88" t="n">
+        <v>0</v>
+      </c>
+      <c r="M88" t="n">
+        <v>0</v>
+      </c>
+      <c r="N88" t="n">
         <v>29</v>
       </c>
-      <c r="M88" t="n">
-        <v>0</v>
-      </c>
-      <c r="N88" t="n">
+      <c r="O88" t="n">
+        <v>0</v>
+      </c>
+      <c r="P88" t="n">
         <v>7.865168539325842</v>
       </c>
-      <c r="O88" t="n">
+      <c r="Q88" t="n">
         <v>243</v>
       </c>
     </row>
@@ -5529,27 +6617,33 @@
         <v>-0.6666666666666667</v>
       </c>
       <c r="H89" t="n">
+        <v>14</v>
+      </c>
+      <c r="I89" t="n">
+        <v>9.666666666666666</v>
+      </c>
+      <c r="J89" t="n">
         <v>3</v>
       </c>
-      <c r="I89" t="n">
+      <c r="K89" t="n">
         <v>785</v>
       </c>
-      <c r="J89" t="n">
+      <c r="L89" t="n">
         <v>-0.7</v>
       </c>
-      <c r="K89" t="n">
-        <v>0</v>
-      </c>
-      <c r="L89" t="n">
+      <c r="M89" t="n">
+        <v>0</v>
+      </c>
+      <c r="N89" t="n">
         <v>29</v>
       </c>
-      <c r="M89" t="n">
-        <v>0</v>
-      </c>
-      <c r="N89" t="n">
+      <c r="O89" t="n">
+        <v>0</v>
+      </c>
+      <c r="P89" t="n">
         <v>2.287581699346405</v>
       </c>
-      <c r="O89" t="n">
+      <c r="Q89" t="n">
         <v>247</v>
       </c>
     </row>
@@ -5576,27 +6670,33 @@
         <v>-1</v>
       </c>
       <c r="H90" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="I90" t="n">
+        <v>9.333333333333334</v>
+      </c>
+      <c r="J90" t="n">
         <v>4</v>
       </c>
-      <c r="I90" t="n">
+      <c r="K90" t="n">
         <v>789</v>
       </c>
-      <c r="J90" t="n">
+      <c r="L90" t="n">
         <v>0.3333333333333333</v>
       </c>
-      <c r="K90" t="n">
-        <v>0</v>
-      </c>
-      <c r="L90" t="n">
+      <c r="M90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N90" t="n">
         <v>29</v>
       </c>
-      <c r="M90" t="n">
-        <v>0</v>
-      </c>
-      <c r="N90" t="n">
-        <v>0</v>
-      </c>
       <c r="O90" t="n">
+        <v>0</v>
+      </c>
+      <c r="P90" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q90" t="n">
         <v>243</v>
       </c>
     </row>
@@ -5623,27 +6723,33 @@
         <v>0</v>
       </c>
       <c r="H91" t="n">
+        <v>3</v>
+      </c>
+      <c r="I91" t="n">
+        <v>4.333333333333333</v>
+      </c>
+      <c r="J91" t="n">
         <v>2</v>
       </c>
-      <c r="I91" t="n">
+      <c r="K91" t="n">
         <v>791</v>
       </c>
-      <c r="J91" t="n">
+      <c r="L91" t="n">
         <v>-0.5</v>
       </c>
-      <c r="K91" t="n">
+      <c r="M91" t="n">
         <v>1</v>
       </c>
-      <c r="L91" t="n">
+      <c r="N91" t="n">
         <v>30</v>
       </c>
-      <c r="M91" t="n">
-        <v>0</v>
-      </c>
-      <c r="N91" t="n">
+      <c r="O91" t="n">
+        <v>0</v>
+      </c>
+      <c r="P91" t="n">
         <v>2.469135802469136</v>
       </c>
-      <c r="O91" t="n">
+      <c r="Q91" t="n">
         <v>247</v>
       </c>
     </row>
@@ -5670,27 +6776,33 @@
         <v>0.5</v>
       </c>
       <c r="H92" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="I92" t="n">
+        <v>5</v>
+      </c>
+      <c r="J92" t="n">
         <v>3</v>
       </c>
-      <c r="I92" t="n">
+      <c r="K92" t="n">
         <v>794</v>
       </c>
-      <c r="J92" t="n">
+      <c r="L92" t="n">
         <v>0.5</v>
       </c>
-      <c r="K92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L92" t="n">
+      <c r="M92" t="n">
+        <v>0</v>
+      </c>
+      <c r="N92" t="n">
         <v>30</v>
       </c>
-      <c r="M92" t="n">
+      <c r="O92" t="n">
         <v>-1</v>
       </c>
-      <c r="N92" t="n">
+      <c r="P92" t="n">
         <v>4.090909090909091</v>
       </c>
-      <c r="O92" t="n">
+      <c r="Q92" t="n">
         <v>253</v>
       </c>
     </row>
@@ -5717,27 +6829,33 @@
         <v>-0.8888888888888888</v>
       </c>
       <c r="H93" t="n">
+        <v>5</v>
+      </c>
+      <c r="I93" t="n">
+        <v>5.333333333333333</v>
+      </c>
+      <c r="J93" t="n">
         <v>7</v>
       </c>
-      <c r="I93" t="n">
+      <c r="K93" t="n">
         <v>801</v>
       </c>
-      <c r="J93" t="n">
+      <c r="L93" t="n">
         <v>1.333333333333333</v>
       </c>
-      <c r="K93" t="n">
-        <v>0</v>
-      </c>
-      <c r="L93" t="n">
+      <c r="M93" t="n">
+        <v>0</v>
+      </c>
+      <c r="N93" t="n">
         <v>30</v>
       </c>
-      <c r="M93" t="n">
-        <v>0</v>
-      </c>
-      <c r="N93" t="n">
+      <c r="O93" t="n">
+        <v>0</v>
+      </c>
+      <c r="P93" t="n">
         <v>0.3745318352059925</v>
       </c>
-      <c r="O93" t="n">
+      <c r="Q93" t="n">
         <v>247</v>
       </c>
     </row>

</xml_diff>